<commit_message>
switched places between obj func and constraint, finally outputting!!!!
</commit_message>
<xml_diff>
--- a/result1_86.xlsx
+++ b/result1_86.xlsx
@@ -139,142 +139,142 @@
     <t>菠菜</t>
   </si>
   <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 20.0, 'D3': 0.0, 'D4': 12.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 20.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 30.0, 'D2': 0.0, 'D3': 28.0, 'D4': 0.0, 'D5': 20.0, 'D6': 24.0, 'D7': 22.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 1.2, 'E8': 1.2, 'E9': 0.0, 'E10': 1.2, 'E11': 0.0, 'E12': 1.2, 'E13': 0.0, 'E14': 0.0, 'E15': 1.2, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 1.2, 'E2': 0.0, 'E3': 0.0, 'E4': 1.2, 'E5': 1.2, 'E6': 1.2, 'E7': 0.0, 'E8': 0.0, 'E9': 1.2, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 1.2, 'E3': 1.2, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 1.2, 'E12': 0.0, 'E13': 0.0, 'E14': 1.2, 'E15': 0.0, 'E16': 1.2, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 1.2, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 1.2, 'F2': 1.2, 'F3': 1.2, 'F4': 1.2}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 4.5, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 6.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 20.4, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 12.0, 'D5': 20.0, 'D6': 0.0, 'D7': 0.0, 'D8': 20.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 30.0, 'D2': 20.0, 'D3': 28.0, 'D4': 0.0, 'D5': 0.0, 'D6': 24.0, 'D7': 22.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 1.2, 'E6': 0.0, 'E7': 0.0, 'E8': 1.2, 'E9': 1.2, 'E10': 0.0, 'E11': 1.2, 'E12': 0.0, 'E13': 0.0, 'E14': 1.2, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 1.2, 'E3': 0.0, 'E4': 1.2, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 1.2, 'E13': 1.2, 'E14': 0.0, 'E15': 0.0, 'E16': 1.2, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 1.2, 'E2': 0.0, 'E3': 1.2, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 1.2, 'E8': 0.0, 'E9': 0.0, 'E10': 1.2, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 1.2, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 1.2, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 1.2, 'F2': 1.2, 'F3': 1.2, 'F4': 1.2}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 16.5, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 16.5, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 8.1, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 18.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 4.5, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 13.8, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 1.2, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 1.2, 'E8': 1.2, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 1.2, 'E13': 0.0, 'E14': 1.2, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 13.2, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 1.2, 'E3': 0.0, 'E4': 1.2, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 1.2, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 1.2, 'E14': 0.0, 'E15': 0.0, 'E16': 1.2, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 1.2, 'E4': 0.0, 'E5': 1.2, 'E6': 1.2, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 1.2, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 1.2, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 1.2, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 1.2, 'F2': 1.2, 'F3': 1.2, 'F4': 1.2}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 20.0, 'D3': 0.0, 'D4': 12.0, 'D5': 20.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 30.0, 'D2': 0.0, 'D3': 28.0, 'D4': 0.0, 'D5': 0.0, 'D6': 24.0, 'D7': 22.0, 'D8': 20.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 1.2, 'E6': 0.0, 'E7': 0.0, 'E8': 1.2, 'E9': 1.2, 'E10': 0.0, 'E11': 1.2, 'E12': 0.0, 'E13': 1.2, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 1.2, 'E2': 0.0, 'E3': 0.0, 'E4': 1.2, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 1.2, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 1.2, 'E16': 1.2, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 1.2, 'E3': 1.2, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 1.2, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 1.2, 'E13': 0.0, 'E14': 1.2, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 21.6, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 16.5, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 1.2, 'E2': 0.0, 'E3': 0.0, 'E4': 1.2, 'E5': 0.0, 'E6': 1.2, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 1.2, 'E15': 0.0, 'E16': 1.2, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 7.5, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 4.5, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 1.2, 'E6': 0.0, 'E7': 1.2, 'E8': 0.0, 'E9': 1.2, 'E10': 1.2, 'E11': 1.2, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 1.2, 'E3': 1.2, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 1.2, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 1.2, 'E13': 1.2, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 1.2, 'E16': 0.0, 'F1': 1.2, 'F2': 1.2, 'F3': 1.2, 'F4': 1.2}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 25.8, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 8.4, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 10.5, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 1.2, 'E4': 1.2, 'E5': 0.0, 'E6': 1.2, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 1.2, 'E13': 1.2, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 1.2, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 1.2, 'E11': 1.2, 'E12': 0.0, 'E13': 0.0, 'E14': 1.2, 'E15': 0.0, 'E16': 1.2, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 1.2, 'E2': 1.2, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 1.2, 'E9': 1.2, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 1.2, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 1.2, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 1.2, 'F2': 1.2, 'F3': 1.2, 'F4': 1.2}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 1.2, 'E4': 1.2, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 1.2, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 1.2, 'E13': 0.0, 'E14': 0.0, 'E15': 1.2, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 1.2, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 1.2, 'E7': 0.0, 'E8': 0.0, 'E9': 1.2, 'E10': 0.0, 'E11': 1.2, 'E12': 0.0, 'E13': 0.0, 'E14': 1.2, 'E15': 0.0, 'E16': 0.0, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 0.0, 'E3': 0.0, 'E4': 0.0, 'E5': 1.2, 'E6': 0.0, 'E7': 1.2, 'E8': 0.0, 'E9': 0.0, 'E10': 1.2, 'E11': 0.0, 'E12': 0.0, 'E13': 1.2, 'E14': 0.0, 'E15': 0.0, 'E16': 1.2, 'F1': 0.0, 'F2': 0.0, 'F3': 0.0, 'F4': 0.0}</t>
-  </si>
-  <si>
-    <t>{'A1': 0.0, 'A2': 0.0, 'A3': 0.0, 'A4': 0.0, 'A5': 0.0, 'A6': 0.0, 'B1': 0.0, 'B2': 0.0, 'B3': 0.0, 'B4': 0.0, 'B5': 0.0, 'B6': 0.0, 'B7': 0.0, 'B8': 0.0, 'B9': 0.0, 'B10': 0.0, 'B11': 0.0, 'B12': 0.0, 'B13': 0.0, 'B14': 0.0, 'C1': 0.0, 'C2': 0.0, 'C3': 0.0, 'C4': 0.0, 'C5': 0.0, 'C6': 0.0, 'D1': 0.0, 'D2': 0.0, 'D3': 0.0, 'D4': 0.0, 'D5': 0.0, 'D6': 0.0, 'D7': 0.0, 'D8': 0.0, 'E1': 0.0, 'E2': 1.2, 'E3': 0.0, 'E4': 0.0, 'E5': 0.0, 'E6': 0.0, 'E7': 0.0, 'E8': 0.0, 'E9': 0.0, 'E10': 0.0, 'E11': 0.0, 'E12': 0.0, 'E13': 0.0, 'E14': 0.0, 'E15': 0.0, 'E16': 0.0, 'F1': 1.2, 'F2': 1.2, 'F3': 1.2, 'F4': 1.2}</t>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 20.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 12.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 20.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 30.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 28.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 20.0}, 'D6': {'第二季': 24.0}, 'D7': {'第二季': 22.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 1.2}, 'E8': {'第二季': 1.2}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 1.2}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 1.2}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 1.2}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 1.2}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 1.2}, 'E5': {'第二季': 1.2}, 'E6': {'第二季': 1.2}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 1.2}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 1.2}, 'E3': {'第二季': 1.2}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 1.2}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 1.2}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 1.2}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 1.2}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 1.2}, 'F2': {'第二季': 1.2}, 'F3': {'第二季': 1.2}, 'F4': {'第二季': 1.2}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 4.5}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 6.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 20.4}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 12.0}, 'D5': {'第二季': 20.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 20.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 30.0}, 'D2': {'第二季': 20.0}, 'D3': {'第二季': 28.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 24.0}, 'D7': {'第二季': 22.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 1.2}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 1.2}, 'E9': {'第二季': 1.2}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 1.2}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 1.2}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 1.2}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 1.2}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 1.2}, 'E13': {'第二季': 1.2}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 1.2}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 1.2}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 1.2}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 1.2}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 1.2}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 1.2}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 1.2}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 1.2}, 'F2': {'第二季': 1.2}, 'F3': {'第二季': 1.2}, 'F4': {'第二季': 1.2}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 16.5}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 16.5}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 8.1}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 18.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 4.5}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 13.8}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 1.2}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 1.2}, 'E8': {'第二季': 1.2}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 1.2}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 1.2}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 13.2}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 1.2}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 1.2}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 1.2}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 1.2}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 1.2}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 1.2}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 1.2}, 'E6': {'第二季': 1.2}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 1.2}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 1.2}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 1.2}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 1.2}, 'F2': {'第二季': 1.2}, 'F3': {'第二季': 1.2}, 'F4': {'第二季': 1.2}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 20.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 12.0}, 'D5': {'第二季': 20.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 30.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 28.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 24.0}, 'D7': {'第二季': 22.0}, 'D8': {'第二季': 20.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 1.2}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 1.2}, 'E9': {'第二季': 1.2}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 1.2}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 1.2}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 1.2}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 1.2}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 1.2}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 1.2}, 'E16': {'第二季': 1.2}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 1.2}, 'E3': {'第二季': 1.2}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 1.2}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 1.2}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 1.2}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 21.6}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 16.5}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 1.2}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 1.2}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 1.2}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 1.2}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 1.2}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 7.5}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 4.5}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 1.2}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 1.2}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 1.2}, 'E10': {'第二季': 1.2}, 'E11': {'第二季': 1.2}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 1.2}, 'E3': {'第二季': 1.2}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 1.2}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 1.2}, 'E13': {'第二季': 1.2}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 1.2}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 1.2}, 'F2': {'第二季': 1.2}, 'F3': {'第二季': 1.2}, 'F4': {'第二季': 1.2}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 25.8}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 8.4}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 10.5}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 1.2}, 'E4': {'第二季': 1.2}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 1.2}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 1.2}, 'E13': {'第二季': 1.2}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 1.2}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 1.2}, 'E11': {'第二季': 1.2}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 1.2}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 1.2}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 1.2}, 'E2': {'第二季': 1.2}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 1.2}, 'E9': {'第二季': 1.2}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 1.2}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 1.2}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 1.2}, 'F2': {'第二季': 1.2}, 'F3': {'第二季': 1.2}, 'F4': {'第二季': 1.2}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 1.2}, 'E4': {'第二季': 1.2}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 1.2}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 1.2}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 1.2}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 1.2}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 1.2}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 1.2}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 1.2}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 1.2}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 0.0}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 1.2}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 1.2}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 1.2}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 1.2}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 1.2}, 'F1': {'第二季': 0.0}, 'F2': {'第二季': 0.0}, 'F3': {'第二季': 0.0}, 'F4': {'第二季': 0.0}}</t>
+  </si>
+  <si>
+    <t>{'A1': {'第二季': 0.0}, 'A2': {'第二季': 0.0}, 'A3': {'第二季': 0.0}, 'A4': {'第二季': 0.0}, 'A5': {'第二季': 0.0}, 'A6': {'第二季': 0.0}, 'B1': {'第二季': 0.0}, 'B2': {'第二季': 0.0}, 'B3': {'第二季': 0.0}, 'B4': {'第二季': 0.0}, 'B5': {'第二季': 0.0}, 'B6': {'第二季': 0.0}, 'B7': {'第二季': 0.0}, 'B8': {'第二季': 0.0}, 'B9': {'第二季': 0.0}, 'B10': {'第二季': 0.0}, 'B11': {'第二季': 0.0}, 'B12': {'第二季': 0.0}, 'B13': {'第二季': 0.0}, 'B14': {'第二季': 0.0}, 'C1': {'第二季': 0.0}, 'C2': {'第二季': 0.0}, 'C3': {'第二季': 0.0}, 'C4': {'第二季': 0.0}, 'C5': {'第二季': 0.0}, 'C6': {'第二季': 0.0}, 'D1': {'第二季': 0.0}, 'D2': {'第二季': 0.0}, 'D3': {'第二季': 0.0}, 'D4': {'第二季': 0.0}, 'D5': {'第二季': 0.0}, 'D6': {'第二季': 0.0}, 'D7': {'第二季': 0.0}, 'D8': {'第二季': 0.0}, 'E1': {'第二季': 0.0}, 'E2': {'第二季': 1.2}, 'E3': {'第二季': 0.0}, 'E4': {'第二季': 0.0}, 'E5': {'第二季': 0.0}, 'E6': {'第二季': 0.0}, 'E7': {'第二季': 0.0}, 'E8': {'第二季': 0.0}, 'E9': {'第二季': 0.0}, 'E10': {'第二季': 0.0}, 'E11': {'第二季': 0.0}, 'E12': {'第二季': 0.0}, 'E13': {'第二季': 0.0}, 'E14': {'第二季': 0.0}, 'E15': {'第二季': 0.0}, 'E16': {'第二季': 0.0}, 'F1': {'第二季': 1.2}, 'F2': {'第二季': 1.2}, 'F3': {'第二季': 1.2}, 'F4': {'第二季': 1.2}}</t>
   </si>
 </sst>
 </file>

</xml_diff>